<commit_message>
metadata option added and handled
</commit_message>
<xml_diff>
--- a/sample_smiles.xlsx
+++ b/sample_smiles.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="26">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -28,7 +28,19 @@
     <t xml:space="preserve">structure</t>
   </si>
   <si>
+    <t xml:space="preserve">meta1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meta2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meta3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cc1ccc(Cl)cc1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy</t>
   </si>
   <si>
     <t xml:space="preserve">NC#N</t>
@@ -201,10 +213,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -221,165 +233,354 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>131</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>513</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>79</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>622</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>736</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>785</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>743</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>804</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>512</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>996</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>1013</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>1065</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>987</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>1159</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>455</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>738</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>974</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>417</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>1049</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>24</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>695</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>